<commit_message>
Add function to get the estimations for the stocks
</commit_message>
<xml_diff>
--- a/doc/Equity Bond Analisis Veeva.xlsx
+++ b/doc/Equity Bond Analisis Veeva.xlsx
@@ -65,7 +65,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.00[$$]"/>
     <numFmt numFmtId="167" formatCode="0.00\ %"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -125,6 +125,14 @@
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
@@ -184,7 +192,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -235,6 +243,10 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -343,9 +355,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>174240</xdr:colOff>
+      <xdr:colOff>173880</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>25920</xdr:rowOff>
+      <xdr:rowOff>25560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -358,8 +370,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7209000" y="399960"/>
-          <a:ext cx="3671280" cy="1627920"/>
+          <a:off x="7219080" y="399960"/>
+          <a:ext cx="3675960" cy="1627560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -380,9 +392,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>450720</xdr:colOff>
+      <xdr:colOff>450360</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>136440</xdr:rowOff>
+      <xdr:rowOff>173520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -395,8 +407,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7161480" y="2177280"/>
-          <a:ext cx="3995280" cy="3028320"/>
+          <a:off x="7171560" y="2177280"/>
+          <a:ext cx="3999960" cy="3027960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -416,18 +428,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>44789</v>
+        <v>44791</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -444,7 +456,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="4" t="n">
-        <v>229.83</v>
+        <v>223.88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -596,7 +608,7 @@
         <v>5.19</v>
       </c>
       <c r="F12" s="10" t="n">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="G12" s="10"/>
     </row>
@@ -647,7 +659,7 @@
       </c>
       <c r="F15" s="9" t="n">
         <f aca="false">F12*F9</f>
-        <v>3458.45</v>
+        <v>20750.7</v>
       </c>
       <c r="G15" s="9"/>
     </row>
@@ -674,7 +686,7 @@
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F18" s="11" t="n">
         <f aca="false">((F15/G3)^(1/10))-1</f>
-        <v>0.311437138997624</v>
+        <v>0.572902292245754</v>
       </c>
       <c r="G18" s="11"/>
     </row>
@@ -703,6 +715,9 @@
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G23" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>